<commit_message>
ReservationDeetail, ReservationContact, My Reservation
</commit_message>
<xml_diff>
--- a/GroupXX_ChidrenCare_Final Product Backlog.xlsx
+++ b/GroupXX_ChidrenCare_Final Product Backlog.xlsx
@@ -3668,7 +3668,7 @@
   <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="117" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -3809,27 +3809,27 @@
         <f>ROW()-9</f>
         <v>-5</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
+      <c r="B4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E4" s="13">
-        <f t="shared" ref="E4:E38" si="0">IF(D4="Complex", 240, IF(D4="Medium",120,60))</f>
-        <v>120</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>137</v>
+        <f>IF(D4="Complex", 240, IF(D4="Medium",120,60))</f>
+        <v>60</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>151</v>
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
@@ -3839,39 +3839,39 @@
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
-      <c r="Q4" s="6" t="s">
-        <v>137</v>
+      <c r="Q4" s="8" t="s">
+        <v>151</v>
       </c>
       <c r="R4" s="17"/>
       <c r="S4" s="17"/>
       <c r="T4" s="17"/>
     </row>
-    <row r="5" spans="1:20" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="153" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <f t="shared" ref="A5:A38" si="1">ROW()-9</f>
+        <f>ROW()-9</f>
         <v>-4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>5</v>
+      <c r="B5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="13">
-        <f t="shared" si="0"/>
+        <f>IF(D5="Complex", 240, IF(D5="Medium",120,60))</f>
         <v>60</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>138</v>
+      <c r="F5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>152</v>
       </c>
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
@@ -3881,39 +3881,39 @@
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
-      <c r="Q5" s="6" t="s">
-        <v>138</v>
+      <c r="Q5" s="8" t="s">
+        <v>152</v>
       </c>
       <c r="R5" s="17"/>
       <c r="S5" s="17"/>
       <c r="T5" s="17"/>
     </row>
-    <row r="6" spans="1:20" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>-3</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>5</v>
+      <c r="B6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="13">
-        <f t="shared" si="0"/>
+        <f>IF(D6="Complex", 240, IF(D6="Medium",120,60))</f>
         <v>60</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>139</v>
+      <c r="F6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
@@ -3923,8 +3923,8 @@
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
-      <c r="Q6" s="6" t="s">
-        <v>139</v>
+      <c r="Q6" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="R6" s="17"/>
       <c r="S6" s="17"/>
@@ -3932,30 +3932,30 @@
     </row>
     <row r="7" spans="1:20" ht="149.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>-2</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
+      <c r="B7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E7" s="13">
-        <f t="shared" si="0"/>
-        <v>240</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>140</v>
+        <f>IF(D7="Complex", 240, IF(D7="Medium",120,60))</f>
+        <v>60</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
@@ -3965,8 +3965,8 @@
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
       <c r="P7" s="17"/>
-      <c r="Q7" s="6" t="s">
-        <v>140</v>
+      <c r="Q7" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="R7" s="17"/>
       <c r="S7" s="17"/>
@@ -3974,30 +3974,30 @@
     </row>
     <row r="8" spans="1:20" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>-1</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>5</v>
+      <c r="B8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E8" s="13">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>141</v>
+        <f>IF(D8="Complex", 240, IF(D8="Medium",120,60))</f>
+        <v>60</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>101</v>
       </c>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
@@ -4007,8 +4007,8 @@
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
-      <c r="Q8" s="6" t="s">
-        <v>141</v>
+      <c r="Q8" s="8" t="s">
+        <v>101</v>
       </c>
       <c r="R8" s="17"/>
       <c r="S8" s="17"/>
@@ -4016,34 +4016,32 @@
     </row>
     <row r="9" spans="1:20" ht="143.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>0</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>5</v>
+      <c r="B9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E9" s="13">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G9" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="H9" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>153</v>
-      </c>
+        <f>IF(D9="Complex", 240, IF(D9="Medium",120,60))</f>
+        <v>60</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I9" s="17"/>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
@@ -4051,8 +4049,8 @@
       <c r="N9" s="17"/>
       <c r="O9" s="17"/>
       <c r="P9" s="17"/>
-      <c r="Q9" s="32" t="s">
-        <v>142</v>
+      <c r="Q9" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
@@ -4060,34 +4058,32 @@
     </row>
     <row r="10" spans="1:20" ht="167.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>1</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>5</v>
+      <c r="B10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E10" s="13">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>153</v>
-      </c>
+        <f>IF(D10="Complex", 240, IF(D10="Medium",120,60))</f>
+        <v>60</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="17"/>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
@@ -4095,8 +4091,8 @@
       <c r="N10" s="17"/>
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
-      <c r="Q10" s="6" t="s">
-        <v>146</v>
+      <c r="Q10" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="R10" s="17"/>
       <c r="S10" s="17"/>
@@ -4104,34 +4100,32 @@
     </row>
     <row r="11" spans="1:20" ht="177.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>2</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>5</v>
+      <c r="B11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E11" s="13">
-        <f t="shared" si="0"/>
-        <v>240</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="I11" s="33" t="s">
-        <v>153</v>
-      </c>
+        <f>IF(D11="Complex", 240, IF(D11="Medium",120,60))</f>
+        <v>120</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I11" s="17"/>
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
@@ -4139,8 +4133,8 @@
       <c r="N11" s="17"/>
       <c r="O11" s="17"/>
       <c r="P11" s="17"/>
-      <c r="Q11" s="6" t="s">
-        <v>143</v>
+      <c r="Q11" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="R11" s="17"/>
       <c r="S11" s="17"/>
@@ -4148,30 +4142,30 @@
     </row>
     <row r="12" spans="1:20" ht="138.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>3</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>5</v>
+      <c r="B12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="13">
-        <f t="shared" si="0"/>
+        <f>IF(D12="Complex", 240, IF(D12="Medium",120,60))</f>
         <v>60</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>144</v>
+      <c r="F12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
@@ -4181,8 +4175,8 @@
       <c r="N12" s="17"/>
       <c r="O12" s="17"/>
       <c r="P12" s="17"/>
-      <c r="Q12" s="6" t="s">
-        <v>144</v>
+      <c r="Q12" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="R12" s="17"/>
       <c r="S12" s="17"/>
@@ -4190,11 +4184,11 @@
     </row>
     <row r="13" spans="1:20" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>4</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>13</v>
@@ -4203,17 +4197,17 @@
         <v>8</v>
       </c>
       <c r="E13" s="13">
-        <f t="shared" si="0"/>
+        <f>IF(D13="Complex", 240, IF(D13="Medium",120,60))</f>
         <v>60</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
@@ -4224,38 +4218,38 @@
       <c r="O13" s="17"/>
       <c r="P13" s="17"/>
       <c r="Q13" s="8" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="R13" s="17"/>
       <c r="S13" s="17"/>
       <c r="T13" s="17"/>
     </row>
-    <row r="14" spans="1:20" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>5</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="B14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="13">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>84</v>
+      <c r="D14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="14">
+        <f>IF(D14="Complex", 240, IF(D14="Medium",120,60))</f>
+        <v>240</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="I14" s="17"/>
       <c r="J14" s="17"/>
@@ -4265,8 +4259,8 @@
       <c r="N14" s="17"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
-      <c r="Q14" s="8" t="s">
-        <v>84</v>
+      <c r="Q14" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="R14" s="17"/>
       <c r="S14" s="17"/>
@@ -4274,30 +4268,30 @@
     </row>
     <row r="15" spans="1:20" ht="102" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>6</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E15" s="13">
-        <f t="shared" si="0"/>
-        <v>120</v>
+        <f>IF(D15="Complex", 240, IF(D15="Medium",120,60))</f>
+        <v>60</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
@@ -4308,40 +4302,42 @@
       <c r="O15" s="17"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="8" t="s">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="R15" s="17"/>
       <c r="S15" s="17"/>
       <c r="T15" s="17"/>
     </row>
-    <row r="16" spans="1:20" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>7</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E16" s="13">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I16" s="17"/>
+        <f>IF(D16="Complex", 240, IF(D16="Medium",120,60))</f>
+        <v>120</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>153</v>
+      </c>
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
@@ -4349,39 +4345,39 @@
       <c r="N16" s="17"/>
       <c r="O16" s="17"/>
       <c r="P16" s="17"/>
-      <c r="Q16" s="8" t="s">
-        <v>86</v>
+      <c r="Q16" s="12" t="s">
+        <v>147</v>
       </c>
       <c r="R16" s="17"/>
       <c r="S16" s="17"/>
       <c r="T16" s="17"/>
     </row>
-    <row r="17" spans="1:20" ht="51" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>8</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E17" s="13">
-        <f t="shared" si="0"/>
-        <v>60</v>
+        <f>IF(D17="Complex", 240, IF(D17="Medium",120,60))</f>
+        <v>120</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
@@ -4392,38 +4388,38 @@
       <c r="O17" s="17"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="R17" s="17"/>
       <c r="S17" s="17"/>
       <c r="T17" s="17"/>
     </row>
-    <row r="18" spans="1:20" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="51" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>9</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="14">
-        <f t="shared" si="0"/>
-        <v>240</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>88</v>
+      <c r="B18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="13">
+        <f>IF(D18="Complex", 240, IF(D18="Medium",120,60))</f>
+        <v>120</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="I18" s="17"/>
       <c r="J18" s="17"/>
@@ -4433,39 +4429,39 @@
       <c r="N18" s="17"/>
       <c r="O18" s="17"/>
       <c r="P18" s="17"/>
-      <c r="Q18" s="11" t="s">
-        <v>88</v>
+      <c r="Q18" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="R18" s="17"/>
       <c r="S18" s="17"/>
       <c r="T18" s="17"/>
     </row>
-    <row r="19" spans="1:20" ht="102" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>10</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>117</v>
+        <v>28</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="13">
-        <f t="shared" si="0"/>
+        <f>IF(D19="Complex", 240, IF(D19="Medium",120,60))</f>
         <v>60</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>118</v>
+        <v>29</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>145</v>
+        <v>91</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>145</v>
+        <v>91</v>
       </c>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
@@ -4476,7 +4472,7 @@
       <c r="O19" s="17"/>
       <c r="P19" s="17"/>
       <c r="Q19" s="8" t="s">
-        <v>145</v>
+        <v>91</v>
       </c>
       <c r="R19" s="17"/>
       <c r="S19" s="17"/>
@@ -4484,34 +4480,32 @@
     </row>
     <row r="20" spans="1:20" ht="162.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>11</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>119</v>
+        <v>30</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E20" s="13">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="I20" s="33" t="s">
-        <v>153</v>
-      </c>
+        <f>IF(D20="Complex", 240, IF(D20="Medium",120,60))</f>
+        <v>60</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" s="17"/>
       <c r="J20" s="17"/>
       <c r="K20" s="17"/>
       <c r="L20" s="17"/>
@@ -4519,8 +4513,8 @@
       <c r="N20" s="17"/>
       <c r="O20" s="17"/>
       <c r="P20" s="17"/>
-      <c r="Q20" s="12" t="s">
-        <v>147</v>
+      <c r="Q20" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="R20" s="17"/>
       <c r="S20" s="17"/>
@@ -4528,11 +4522,11 @@
     </row>
     <row r="21" spans="1:20" ht="81.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>12</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>121</v>
@@ -4541,17 +4535,17 @@
         <v>6</v>
       </c>
       <c r="E21" s="13">
-        <f t="shared" si="0"/>
+        <f>IF(D21="Complex", 240, IF(D21="Medium",120,60))</f>
         <v>120</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>25</v>
+        <v>122</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
@@ -4562,7 +4556,7 @@
       <c r="O21" s="17"/>
       <c r="P21" s="17"/>
       <c r="Q21" s="8" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="R21" s="17"/>
       <c r="S21" s="17"/>
@@ -4570,11 +4564,11 @@
     </row>
     <row r="22" spans="1:20" ht="75.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>13</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>26</v>
+        <v>107</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>121</v>
@@ -4583,17 +4577,17 @@
         <v>6</v>
       </c>
       <c r="E22" s="13">
-        <f t="shared" si="0"/>
+        <f>IF(D22="Complex", 240, IF(D22="Medium",120,60))</f>
         <v>120</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>27</v>
+        <v>123</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
@@ -4604,19 +4598,19 @@
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="R22" s="17"/>
       <c r="S22" s="17"/>
       <c r="T22" s="17"/>
     </row>
-    <row r="23" spans="1:20" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>14</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>121</v>
@@ -4625,17 +4619,17 @@
         <v>8</v>
       </c>
       <c r="E23" s="13">
-        <f t="shared" si="0"/>
+        <f>IF(D23="Complex", 240, IF(D23="Medium",120,60))</f>
         <v>60</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="I23" s="17"/>
       <c r="J23" s="17"/>
@@ -4646,7 +4640,7 @@
       <c r="O23" s="17"/>
       <c r="P23" s="17"/>
       <c r="Q23" s="8" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="R23" s="17"/>
       <c r="S23" s="17"/>
@@ -4654,11 +4648,11 @@
     </row>
     <row r="24" spans="1:20" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>15</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>121</v>
@@ -4667,19 +4661,21 @@
         <v>8</v>
       </c>
       <c r="E24" s="13">
-        <f t="shared" si="0"/>
+        <f>IF(D24="Complex", 240, IF(D24="Medium",120,60))</f>
         <v>60</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I24" s="17"/>
+        <v>96</v>
+      </c>
+      <c r="I24" s="33" t="s">
+        <v>153</v>
+      </c>
       <c r="J24" s="17"/>
       <c r="K24" s="17"/>
       <c r="L24" s="17"/>
@@ -4688,19 +4684,19 @@
       <c r="O24" s="17"/>
       <c r="P24" s="17"/>
       <c r="Q24" s="8" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="R24" s="17"/>
       <c r="S24" s="17"/>
       <c r="T24" s="17"/>
     </row>
-    <row r="25" spans="1:20" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>16</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>105</v>
+        <v>36</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>121</v>
@@ -4709,17 +4705,17 @@
         <v>6</v>
       </c>
       <c r="E25" s="13">
-        <f t="shared" si="0"/>
+        <f>IF(D25="Complex", 240, IF(D25="Medium",120,60))</f>
         <v>120</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="I25" s="17"/>
       <c r="J25" s="17"/>
@@ -4730,7 +4726,7 @@
       <c r="O25" s="17"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="8" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="R25" s="17"/>
       <c r="S25" s="17"/>
@@ -4738,32 +4734,34 @@
     </row>
     <row r="26" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>17</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>121</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E26" s="13">
-        <f t="shared" si="0"/>
-        <v>120</v>
+        <f>IF(D26="Complex", 240, IF(D26="Medium",120,60))</f>
+        <v>60</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="I26" s="17"/>
+        <v>98</v>
+      </c>
+      <c r="I26" s="33" t="s">
+        <v>153</v>
+      </c>
       <c r="J26" s="17"/>
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
@@ -4772,7 +4770,7 @@
       <c r="O26" s="17"/>
       <c r="P26" s="17"/>
       <c r="Q26" s="8" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="R26" s="17"/>
       <c r="S26" s="17"/>
@@ -4780,30 +4778,30 @@
     </row>
     <row r="27" spans="1:20" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>18</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>121</v>
+      <c r="B27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E27" s="13">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>95</v>
+        <f>IF(D27="Complex", 240, IF(D27="Medium",120,60))</f>
+        <v>120</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
@@ -4813,8 +4811,8 @@
       <c r="N27" s="17"/>
       <c r="O27" s="17"/>
       <c r="P27" s="17"/>
-      <c r="Q27" s="8" t="s">
-        <v>95</v>
+      <c r="Q27" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="R27" s="17"/>
       <c r="S27" s="17"/>
@@ -4822,34 +4820,32 @@
     </row>
     <row r="28" spans="1:20" ht="123.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>19</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>121</v>
+      <c r="B28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="13">
-        <f t="shared" si="0"/>
+        <f>IF(D28="Complex", 240, IF(D28="Medium",120,60))</f>
         <v>60</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="I28" s="33" t="s">
-        <v>153</v>
-      </c>
+      <c r="F28" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="I28" s="17"/>
       <c r="J28" s="17"/>
       <c r="K28" s="17"/>
       <c r="L28" s="17"/>
@@ -4857,8 +4853,8 @@
       <c r="N28" s="17"/>
       <c r="O28" s="17"/>
       <c r="P28" s="17"/>
-      <c r="Q28" s="8" t="s">
-        <v>96</v>
+      <c r="Q28" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="R28" s="17"/>
       <c r="S28" s="17"/>
@@ -4866,30 +4862,30 @@
     </row>
     <row r="29" spans="1:20" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>20</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>121</v>
+      <c r="B29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E29" s="13">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>97</v>
+        <f>IF(D29="Complex", 240, IF(D29="Medium",120,60))</f>
+        <v>60</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
@@ -4899,8 +4895,8 @@
       <c r="N29" s="17"/>
       <c r="O29" s="17"/>
       <c r="P29" s="17"/>
-      <c r="Q29" s="8" t="s">
-        <v>97</v>
+      <c r="Q29" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="R29" s="17"/>
       <c r="S29" s="17"/>
@@ -4908,34 +4904,32 @@
     </row>
     <row r="30" spans="1:20" ht="81.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>21</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>121</v>
+      <c r="B30" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E30" s="13">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I30" s="33" t="s">
-        <v>153</v>
-      </c>
+        <f>IF(D30="Complex", 240, IF(D30="Medium",120,60))</f>
+        <v>240</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I30" s="17"/>
       <c r="J30" s="17"/>
       <c r="K30" s="17"/>
       <c r="L30" s="17"/>
@@ -4943,8 +4937,8 @@
       <c r="N30" s="17"/>
       <c r="O30" s="17"/>
       <c r="P30" s="17"/>
-      <c r="Q30" s="8" t="s">
-        <v>98</v>
+      <c r="Q30" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="R30" s="17"/>
       <c r="S30" s="17"/>
@@ -4952,34 +4946,32 @@
     </row>
     <row r="31" spans="1:20" ht="150.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>22</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>127</v>
+      <c r="B31" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E31" s="13">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="I31" s="33" t="s">
-        <v>153</v>
-      </c>
+        <f>IF(D31="Complex", 240, IF(D31="Medium",120,60))</f>
+        <v>120</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I31" s="17"/>
       <c r="J31" s="17"/>
       <c r="K31" s="17"/>
       <c r="L31" s="17"/>
@@ -4987,8 +4979,8 @@
       <c r="N31" s="17"/>
       <c r="O31" s="17"/>
       <c r="P31" s="17"/>
-      <c r="Q31" s="8" t="s">
-        <v>148</v>
+      <c r="Q31" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="R31" s="17"/>
       <c r="S31" s="17"/>
@@ -4996,32 +4988,32 @@
     </row>
     <row r="32" spans="1:20" ht="138.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>23</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>127</v>
+      <c r="B32" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E32" s="13">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="I32" s="33" t="s">
+        <f>IF(D32="Complex", 240, IF(D32="Medium",120,60))</f>
+        <v>120</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G32" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="H32" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="I32" s="17" t="s">
         <v>153</v>
       </c>
       <c r="J32" s="17"/>
@@ -5031,8 +5023,8 @@
       <c r="N32" s="17"/>
       <c r="O32" s="17"/>
       <c r="P32" s="17"/>
-      <c r="Q32" s="12" t="s">
-        <v>149</v>
+      <c r="Q32" s="32" t="s">
+        <v>142</v>
       </c>
       <c r="R32" s="17"/>
       <c r="S32" s="17"/>
@@ -5040,32 +5032,34 @@
     </row>
     <row r="33" spans="1:20" ht="122.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>24</v>
       </c>
-      <c r="B33" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="C33" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="D33" s="29" t="s">
+      <c r="B33" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="30">
+      <c r="E33" s="13">
         <f>IF(D33="Complex", 240, IF(D33="Medium",120,60))</f>
         <v>120</v>
       </c>
-      <c r="F33" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G33" s="31" t="s">
-        <v>150</v>
-      </c>
-      <c r="H33" s="31" t="s">
-        <v>150</v>
-      </c>
-      <c r="I33" s="17"/>
+      <c r="F33" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="I33" s="17" t="s">
+        <v>153</v>
+      </c>
       <c r="J33" s="17"/>
       <c r="K33" s="17"/>
       <c r="L33" s="17"/>
@@ -5073,8 +5067,8 @@
       <c r="N33" s="17"/>
       <c r="O33" s="17"/>
       <c r="P33" s="17"/>
-      <c r="Q33" s="31" t="s">
-        <v>150</v>
+      <c r="Q33" s="6" t="s">
+        <v>146</v>
       </c>
       <c r="R33" s="17"/>
       <c r="S33" s="17"/>
@@ -5082,32 +5076,34 @@
     </row>
     <row r="34" spans="1:20" ht="161.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>25</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>39</v>
+      <c r="B34" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E34" s="13">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="I34" s="17"/>
+        <f>IF(D34="Complex", 240, IF(D34="Medium",120,60))</f>
+        <v>240</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="I34" s="33" t="s">
+        <v>153</v>
+      </c>
       <c r="J34" s="17"/>
       <c r="K34" s="17"/>
       <c r="L34" s="17"/>
@@ -5115,8 +5111,8 @@
       <c r="N34" s="17"/>
       <c r="O34" s="17"/>
       <c r="P34" s="17"/>
-      <c r="Q34" s="8" t="s">
-        <v>151</v>
+      <c r="Q34" s="6" t="s">
+        <v>143</v>
       </c>
       <c r="R34" s="17"/>
       <c r="S34" s="17"/>
@@ -5124,30 +5120,30 @@
     </row>
     <row r="35" spans="1:20" ht="101.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>26</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>39</v>
+      <c r="B35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="13">
-        <f t="shared" si="0"/>
+        <f>IF(D35="Complex", 240, IF(D35="Medium",120,60))</f>
         <v>60</v>
       </c>
-      <c r="F35" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>152</v>
+      <c r="F35" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="I35" s="17"/>
       <c r="J35" s="17"/>
@@ -5157,8 +5153,8 @@
       <c r="N35" s="17"/>
       <c r="O35" s="17"/>
       <c r="P35" s="17"/>
-      <c r="Q35" s="8" t="s">
-        <v>152</v>
+      <c r="Q35" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="R35" s="17"/>
       <c r="S35" s="17"/>
@@ -5166,32 +5162,34 @@
     </row>
     <row r="36" spans="1:20" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>27</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>42</v>
+        <v>126</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="13">
-        <f t="shared" si="0"/>
+        <f>IF(D36="Complex", 240, IF(D36="Medium",120,60))</f>
         <v>60</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="I36" s="17"/>
+        <v>148</v>
+      </c>
+      <c r="I36" s="33" t="s">
+        <v>153</v>
+      </c>
       <c r="J36" s="17"/>
       <c r="K36" s="17"/>
       <c r="L36" s="17"/>
@@ -5200,7 +5198,7 @@
       <c r="O36" s="17"/>
       <c r="P36" s="17"/>
       <c r="Q36" s="8" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="R36" s="17"/>
       <c r="S36" s="17"/>
@@ -5208,32 +5206,34 @@
     </row>
     <row r="37" spans="1:20" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>28</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="13">
-        <f t="shared" si="0"/>
+        <f>IF(D37="Complex", 240, IF(D37="Medium",120,60))</f>
         <v>60</v>
       </c>
-      <c r="F37" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="I37" s="17"/>
+      <c r="F37" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="I37" s="33" t="s">
+        <v>153</v>
+      </c>
       <c r="J37" s="17"/>
       <c r="K37" s="17"/>
       <c r="L37" s="17"/>
@@ -5241,8 +5241,8 @@
       <c r="N37" s="17"/>
       <c r="O37" s="17"/>
       <c r="P37" s="17"/>
-      <c r="Q37" s="8" t="s">
-        <v>100</v>
+      <c r="Q37" s="12" t="s">
+        <v>149</v>
       </c>
       <c r="R37" s="17"/>
       <c r="S37" s="17"/>
@@ -5250,30 +5250,30 @@
     </row>
     <row r="38" spans="1:20" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <f t="shared" si="1"/>
+        <f>ROW()-9</f>
         <v>29</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="13">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>101</v>
+      <c r="B38" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="30">
+        <f>IF(D38="Complex", 240, IF(D38="Medium",120,60))</f>
+        <v>120</v>
+      </c>
+      <c r="F38" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G38" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="H38" s="31" t="s">
+        <v>150</v>
       </c>
       <c r="I38" s="17"/>
       <c r="J38" s="17"/>
@@ -5283,15 +5283,19 @@
       <c r="N38" s="17"/>
       <c r="O38" s="17"/>
       <c r="P38" s="17"/>
-      <c r="Q38" s="8" t="s">
-        <v>101</v>
+      <c r="Q38" s="31" t="s">
+        <v>150</v>
       </c>
       <c r="R38" s="17"/>
       <c r="S38" s="17"/>
       <c r="T38" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:ID38"/>
+  <autoFilter ref="A3:ID38">
+    <sortState ref="A4:ID38">
+      <sortCondition ref="C3:C38"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="3">
     <mergeCell ref="H2:M2"/>
     <mergeCell ref="A2:F2"/>

</xml_diff>